<commit_message>
Erweiterung um Erklärung in ganzen Sätzen, also lesbarem Text
</commit_message>
<xml_diff>
--- a/Umlage_Gebaeudeversicherung.xlsx
+++ b/Umlage_Gebaeudeversicherung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99c31bec99ad580a/odc_Dokumente/08_Gewerbe/Kunden/tk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{CFAF7FEB-C488-41DB-8176-11A61ACC4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46B9474A-FC07-4B08-AFD8-1A537F4214A2}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{CFAF7FEB-C488-41DB-8176-11A61ACC4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A9BE5ED-F6CF-4357-931D-3DB54727184E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -93,6 +93,89 @@
   </si>
   <si>
     <t>berechnetes Ergebnis</t>
+  </si>
+  <si>
+    <t>Berechnung eventuelle Ersparnis</t>
+  </si>
+  <si>
+    <t>Vorbereitung</t>
+  </si>
+  <si>
+    <t>Geben Sie die jeweiligen Jahresbeträge der Gebäudeversicherung für das Vorjahr und für das aktuelle Jahr an.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebenso geben Sie die Anzahl der Monate ein, auf die der jeweilige Jahrebetrag entfällt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das hängt ja ab von der jeweiligen Laufzeit des Vertrages, </t>
+  </si>
+  <si>
+    <t>z.B. 01.06. bis 31.05. sind 7 Monate Vorjahr, 5 Monate aktuelles Jahr.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Berücksichtigen Sie, ob der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gesamtbetrag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> der Versicherung bereits im </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vorjahr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> abgerechnet wurde!</t>
+    </r>
+  </si>
+  <si>
+    <t>Ergebnis:</t>
+  </si>
+  <si>
+    <t>Ersparnis</t>
+  </si>
+  <si>
+    <t>12 Monate</t>
+  </si>
+  <si>
+    <t>Anteil für</t>
+  </si>
+  <si>
+    <t>(alte Police)</t>
+  </si>
+  <si>
+    <t>(neue Police)</t>
   </si>
 </sst>
 </file>
@@ -103,7 +186,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="0\ &quot;m²&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +216,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +251,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,12 +338,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -260,13 +363,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Akzent1" xfId="3" builtinId="29"/>
     <cellStyle name="Akzent2" xfId="2" builtinId="33"/>
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -282,6 +396,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -571,20 +689,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -655,7 +776,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -677,14 +798,14 @@
         <f>D9/E9*F9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="16">
         <f>SUM(G9:G10)</f>
         <v>163.20778625954196</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B10" s="11">
         <v>12</v>
@@ -706,7 +827,7 @@
         <f>D10/E10*F10</f>
         <v>163.20778625954196</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="5" t="s">
@@ -784,7 +905,7 @@
         <f>D14/E14*F14</f>
         <v>53.533683206106872</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="16">
         <f>SUM(G14:G15)</f>
         <v>148.73822519083967</v>
       </c>
@@ -813,7 +934,7 @@
         <f>D15/E15*F15</f>
         <v>95.204541984732813</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="5" t="s">
@@ -843,15 +964,13 @@
       </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10">
-        <v>12</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="15"/>
@@ -860,11 +979,9 @@
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B20" s="3">
-        <v>623.37</v>
-      </c>
-      <c r="C20" s="16" t="s">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B20" s="3"/>
+      <c r="C20" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="15"/>
@@ -873,12 +990,9 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="9">
-        <f>G11</f>
-        <v>163.20778625954196</v>
-      </c>
-      <c r="C21" s="16" t="s">
+    <row r="21" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="9"/>
+      <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="15"/>
@@ -887,9 +1001,287 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="17"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="13"/>
+      <c r="B28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="13"/>
+      <c r="B29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="13"/>
+      <c r="B30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="13"/>
+      <c r="B31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="10">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3">
+        <v>623.37</v>
+      </c>
+      <c r="D34" s="2">
+        <f>C34/12*B34</f>
+        <v>259.73750000000001</v>
+      </c>
+      <c r="E34" s="8">
+        <v>262</v>
+      </c>
+      <c r="F34" s="8">
+        <v>54</v>
+      </c>
+      <c r="G34" s="2">
+        <f>D34/E34*F34</f>
+        <v>53.533683206106872</v>
+      </c>
+      <c r="H34" s="16">
+        <f>SUM(G34:G35)</f>
+        <v>148.73822519083967</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11">
+        <v>7</v>
+      </c>
+      <c r="C35" s="4">
+        <v>791.86</v>
+      </c>
+      <c r="D35" s="2">
+        <f>C35/12*B35</f>
+        <v>461.91833333333329</v>
+      </c>
+      <c r="E35" s="8">
+        <v>262</v>
+      </c>
+      <c r="F35" s="8">
+        <v>54</v>
+      </c>
+      <c r="G35" s="2">
+        <f>D35/E35*F35</f>
+        <v>95.204541984732813</v>
+      </c>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:9" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="5">
+        <f>SUM(B34:B35)</f>
+        <v>12</v>
+      </c>
+      <c r="C36" s="6">
+        <f>(B34*C34+B35*C35)/B36</f>
+        <v>721.65583333333336</v>
+      </c>
+      <c r="D36" s="6">
+        <f>C36/12*B36</f>
+        <v>721.65583333333336</v>
+      </c>
+      <c r="E36" s="7">
+        <v>262</v>
+      </c>
+      <c r="F36" s="7">
+        <v>54</v>
+      </c>
+      <c r="G36" s="9">
+        <f>D36/E36*F36</f>
+        <v>148.7382251908397</v>
+      </c>
+      <c r="H36" s="19">
+        <f>G37-G36</f>
+        <v>14.469561068702291</v>
+      </c>
+      <c r="I36" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="G37" s="22">
+        <f>C35/E35*F35</f>
+        <v>163.20778625954199</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="21" t="str">
+        <f>CONCATENATE("Bei einer Aufteilung der Versicherungsbeträge Vorjahr ",TEXT(C34,"#.##0,00 €")," und Abrechnungsjahr ",TEXT(C35,"#.##0,00 €")," ")</f>
+        <v xml:space="preserve">Bei einer Aufteilung der Versicherungsbeträge Vorjahr 623,37 € und Abrechnungsjahr 791,86 € </v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B40" s="21" t="str">
+        <f>CONCATENATE("im Verhältnis ",B34," zu ",B35," Monaten ergibt sich ein Betrag von")</f>
+        <v>im Verhältnis 5 zu 7 Monaten ergibt sich ein Betrag von</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="19">
+        <f>H36</f>
+        <v>14.469561068702291</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B41" s="21" t="str">
+        <f>CONCATENATE("im Vergleich zur vollständigen Abrechnung von ",TEXT(C35,"#.##0,00 €")," im Abrechnungsjahr. ")</f>
+        <v xml:space="preserve">im Vergleich zur vollständigen Abrechnung von 791,86 € im Abrechnungsjahr. </v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B43" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="19">
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C21:H21"/>

</xml_diff>